<commit_message>
add case and getPath
</commit_message>
<xml_diff>
--- a/Layout.xlsx
+++ b/Layout.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\00. Giao duc\01.Cao hoc\99. Luanvan\05.Matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\00. Giao duc\01.Cao hoc\99. Luanvan\05.Matlab\matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C3469F6-C26B-4DF2-850A-CC394DE06D6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA490EB4-C9A8-45C1-9A83-298156664E37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="2" xr2:uid="{25DECE4D-14CB-4F70-B561-1B58AE7016C4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="3" xr2:uid="{25DECE4D-14CB-4F70-B561-1B58AE7016C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
     <sheet name="giai thuat khong xoa" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
   <si>
     <t>Job</t>
   </si>
@@ -225,9 +226,6 @@
     <t>Vòng lặp</t>
   </si>
   <si>
-    <t>Kiểm tra job -&gt; điều phối</t>
-  </si>
-  <si>
     <t>Rerouting</t>
   </si>
   <si>
@@ -331,6 +329,57 @@
   </si>
   <si>
     <t>continue</t>
+  </si>
+  <si>
+    <t>https://repository.up.ac.za/bitstream/handle/2263/62870/vanLoggerenberg_Application_2016.pdf?sequence=1</t>
+  </si>
+  <si>
+    <t>https://sci-hub.se/https://doi.org/10.1007/s00170-013-4775-6</t>
+  </si>
+  <si>
+    <t>http://143.248.80.207/wordpress/wp-content/uploads/2021/04/Predictive-vehicle-dispatching-method-for-overhead-hoist-transport-systems-in-semiconductor-fabs.pdf</t>
+  </si>
+  <si>
+    <t>https://sci-hub.se/10.1109/ICIEEM.2011.6035471</t>
+  </si>
+  <si>
+    <t>https://sci-hub.se/https://doi.org/10.1016/j.compind.2010.10.010</t>
+  </si>
+  <si>
+    <t>dispatching</t>
+  </si>
+  <si>
+    <t>lấy số job cần làm từ trên xuống bằng số xe</t>
+  </si>
+  <si>
+    <t>đổi target cho xe</t>
+  </si>
+  <si>
+    <t>nếu số job &lt; số xe</t>
+  </si>
+  <si>
+    <t>nếu số job=&gt;số xe</t>
+  </si>
+  <si>
+    <t>tính hungarian</t>
+  </si>
+  <si>
+    <t>list xe available là xe idle và retrived not loading</t>
+  </si>
+  <si>
+    <t>list số job cần làm</t>
+  </si>
+  <si>
+    <t>lấy số job bằng số xe</t>
+  </si>
+  <si>
+    <t>Tính ma trận giá trị (danh sách xe ok, danh sách job ok)</t>
+  </si>
+  <si>
+    <t>C_ij = w1. (Tmax-TimeWait) + w2.d_ij</t>
+  </si>
+  <si>
+    <t>https://d1wqtxts1xzle7.cloudfront.net/53549712/s00170-008-1863-020170616-9028-qxdnnr-with-cover-page-v2.pdf?Expires=1648966799&amp;Signature=HuGSUysf1HDmFddv2o21pT~ObvpZP08gWrqcKGNl-s4W7-fgFW9FJ0SYSvQrrFHiPQkJS2bQg2CAOh7xGu9whzaC7gK6oBz-ZLsuEwL-Tii-goMlBA64dCI9fWMQt7kEitdHaOI9V1Eljd1f07RGXONPSlhDtmSTlFiFJr7GXkcs6QxHxtDWQ5g6~pGo1SCrYaWXx1WW3MaQVaKKXoER8G1yYh7Q0H0Ra4iegdxdxkpnJWaGE1YXanSuUUGJk-LGGvXe5-EJCcjOfxvpGJXMW89WHomu-H25Y07vXM41yRHJzQxO7rRv-CAUSGXs3xIoxI2h8JvX3DX3nBLsOQ4dGg__&amp;Key-Pair-Id=APKAJLOHF5GGSLRBV4ZA</t>
   </si>
 </sst>
 </file>
@@ -3059,252 +3108,341 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:Y65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q4" t="s">
+        <v>93</v>
+      </c>
+      <c r="X4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D8" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="R8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
+      <c r="F9" s="13"/>
+      <c r="S9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
+      <c r="R10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="R13" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+      <c r="R14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F16" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F26" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F37" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="4:7" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="4:7" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="4:7" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F50" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4EADB31-C53E-4402-B319-BCAE9C3E828F}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>